<commit_message>
hacer descargables las bases
</commit_message>
<xml_diff>
--- a/utils/cleaners/Equipos y recursos para desarrollar PC (Responses).xlsx
+++ b/utils/cleaners/Equipos y recursos para desarrollar PC (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4062" uniqueCount="925">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2683,6 +2683,120 @@
   </si>
   <si>
     <t>Daniel.cortes.cfk2022@gmail.com</t>
+  </si>
+  <si>
+    <t>Existe una red de internet de claro en  el programa centros digitales pero no funciona se quemo el receptor y la estructura esta dañada</t>
+  </si>
+  <si>
+    <t>El internet es necesario para esta institución y el no tenerlo les limitan muchas capacitaciones a nivel de formación docente cómo para la enseñanza a sus estudiantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existen muchos equipos portátiles pero no existen instalaciones adecuadas para utilizarlos partiendo que la energía con la que se alimenta la institución es solar faltarían más paneles para proveer una mejor fuente de energía </t>
+  </si>
+  <si>
+    <t>No cuentan con infraestructura de Telecomunicaciones</t>
+  </si>
+  <si>
+    <t>Sensores, Soldadura electrónica, Cautines, Pelacables, Pinzas</t>
+  </si>
+  <si>
+    <t>Disponen de un kit STEM</t>
+  </si>
+  <si>
+    <t>No tienen kits desconectados. Cuentan con 1 Kit STEM y las microbits que obtuvieron los docentes, formados en vigencias anteriores.</t>
+  </si>
+  <si>
+    <t>No se cuenta con el servicio de Internet</t>
+  </si>
+  <si>
+    <t>a.nsf.fabian.rincon@cali.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">son portatiles mini </t>
+  </si>
+  <si>
+    <t>placa electronica y placa programable playboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sistema tecpro de norma que llego este año </t>
+  </si>
+  <si>
+    <t>se pueden reproducir hasta 30 ya que se cuenta con fotocopiadora</t>
+  </si>
+  <si>
+    <t>No tiene</t>
+  </si>
+  <si>
+    <t>La IE tiene la infraestructura WIFI pero no hay servicio Internet.</t>
+  </si>
+  <si>
+    <t>No hay computadores</t>
+  </si>
+  <si>
+    <t>Se requiere actualizar los equipos e instalar nuevas aulas de sistemas</t>
+  </si>
+  <si>
+    <t>Las tabletas y los equipos portátiles de computadores para educar fueron robados en el tiempo de la pandemia</t>
+  </si>
+  <si>
+    <t>Existen 6 maletas Handy cricket pero solo hay las fichas lego ya no existen los componentes electrónicos</t>
+  </si>
+  <si>
+    <t>En pocas aulas hay televisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El paquete de oficina se encuentra instalado sólo en algunos computadores. Los que se conectan en la nube no permiten ningún tipo de descarga y limita accesos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La IE cuenta con unos kit de robótica, sin embargo no se logró acceso a ellos para determinar que contienen y su estado. </t>
+  </si>
+  <si>
+    <t>Televisor, Video proyector, Pero no están en la sala, se tienen pero se usan cuando los profesores, 11 televisores, 5 videobeam.</t>
+  </si>
+  <si>
+    <t>Redes eléctricas, Puertos de cableado estructurado para conexión a la red, Convenio alcaldía-ETB para el tema de conectividad pero no funciona.</t>
+  </si>
+  <si>
+    <t>Afirman no tener las micro:bit</t>
+  </si>
+  <si>
+    <t>Al parecer la institución no ha recibido las micro:bit que se entragaron a docentes porque no están en inventario.</t>
+  </si>
+  <si>
+    <t>Un aula de sistemas esta en proceso de adecuación y hay otra funcional</t>
+  </si>
+  <si>
+    <t>Sòlo estan limitados a los equipos de computo y las microbit</t>
+  </si>
+  <si>
+    <t>yessicaeverts@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se acabó el contrato de conexión a internet en el colegio y no se ha renovado. </t>
+  </si>
+  <si>
+    <t>sami123rojare@yahoo.es</t>
+  </si>
+  <si>
+    <t>En la IE, se presenta mala señal de celular y la conectividad es muy deficiente para garantizar conexion a los equipos de computo de la sala.</t>
+  </si>
+  <si>
+    <t>Paquete de diseño gráfico (Ej. Programas de edición de video, edición de mapas de bits, etc), Paquete de software educativo (Ej. cursos de inglés), no se tiene office instalado en los equipos</t>
+  </si>
+  <si>
+    <t>actualmente el docente de tecnologia, esta investigando sobre que programas utilizar en el aula de clase.</t>
+  </si>
+  <si>
+    <t>Tarjetas micro:bit., solo 3 microbits</t>
+  </si>
+  <si>
+    <t>se cuenta con una buena sala de tecnología, pero carece de buena conectividad, en la ie recién instalaron un centro poblado de conectividad pero nunca funciona y no suple la capacidad del numero de estudiantes.</t>
+  </si>
+  <si>
+    <t>solo se encuentran las cartillas que la docente formada ha realizado</t>
+  </si>
+  <si>
+    <t>Existe en la Institución un (1) kit de ruta STEM</t>
   </si>
 </sst>
 </file>
@@ -21260,6 +21374,954 @@
         <v>40</v>
       </c>
     </row>
+    <row r="233">
+      <c r="A233" s="3">
+        <v>44697.486502569445</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C233" s="2">
+        <v>140.0</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F233" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G233" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I233" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="J233" s="2">
+        <v>122.0</v>
+      </c>
+      <c r="K233" s="2">
+        <v>122.0</v>
+      </c>
+      <c r="L233" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="M233" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N233" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O233" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P233" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q233" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="R233" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S233" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="T233" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U233" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V233" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W233" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="X233" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y233" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="Z233" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA233" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB233" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="3">
+        <v>44697.49317667824</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C234" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F234" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G234" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I234" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="J234" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="K234" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="L234" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M234" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N234" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O234" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P234" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R234" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S234" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="T234" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U234" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V234" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W234" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="X234" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="Y234" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="Z234" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA234" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB234" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC234" s="2" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="3">
+        <v>44697.53576863426</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="C235" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F235" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G235" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I235" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="J235" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="K235" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="L235" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M235" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N235" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O235" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P235" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R235" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S235" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="T235" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U235" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V235" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W235" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="X235" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z235" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA235" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB235" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="3">
+        <v>44698.302116990744</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C236" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F236" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="G236" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H236" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J236" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="K236" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="L236" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M236" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N236" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O236" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P236" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q236" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="R236" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V236" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="W236" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="X236" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y236" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="Z236" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA236" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB236" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC236" s="2" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="3">
+        <v>44698.326642141205</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C237" s="2">
+        <v>85.0</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F237" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G237" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H237" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I237" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="J237" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K237" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L237" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M237" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N237" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="O237" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P237" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R237" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V237" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W237" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="X237" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z237" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA237" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB237" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="3">
+        <v>44698.464638958336</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C238" s="2">
+        <v>135.0</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F238" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G238" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H238" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J238" s="2">
+        <v>37.0</v>
+      </c>
+      <c r="K238" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="L238" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N238" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O238" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P238" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q238" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="R238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V238" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W238" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="X238" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y238" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="Z238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB238" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC238" s="2" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="3">
+        <v>44698.627339513885</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C239" s="2">
+        <v>233.0</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F239" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G239" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I239" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="J239" s="2">
+        <v>71.0</v>
+      </c>
+      <c r="K239" s="2">
+        <v>31.0</v>
+      </c>
+      <c r="L239" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M239" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N239" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O239" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P239" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q239" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="R239" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V239" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W239" s="2">
+        <v>28.0</v>
+      </c>
+      <c r="X239" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y239" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="Z239" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA239" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB239" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="3">
+        <v>44699.415555451385</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="C240" s="2">
+        <v>38.0</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F240" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G240" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="J240" s="2">
+        <v>220.0</v>
+      </c>
+      <c r="K240" s="2">
+        <v>184.0</v>
+      </c>
+      <c r="L240" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M240" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N240" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O240" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P240" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R240" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S240" s="2">
+        <v>220.0</v>
+      </c>
+      <c r="T240" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U240" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V240" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="W240" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X240" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y240" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="Z240" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA240" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB240" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="3">
+        <v>44699.435526967594</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C241" s="2">
+        <v>146.0</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F241" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G241" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H241" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I241" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="J241" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="K241" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="L241" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M241" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N241" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O241" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P241" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R241" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V241" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W241" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="X241" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y241" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="Z241" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA241" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB241" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="3">
+        <v>44699.45864196759</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="C242" s="2">
+        <v>194.0</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F242" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G242" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I242" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="J242" s="2">
+        <v>41.0</v>
+      </c>
+      <c r="K242" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="L242" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M242" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N242" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O242" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P242" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R242" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S242" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T242" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U242" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V242" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W242" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="X242" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z242" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA242" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB242" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="3">
+        <v>44699.99359429398</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="C243" s="2">
+        <v>207.0</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F243" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G243" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H243" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I243" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="J243" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="K243" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="L243" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M243" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N243" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O243" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P243" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="Q243" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="R243" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V243" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="W243" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="X243" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y243" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="Z243" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA243" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB243" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC243" s="2" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="3">
+        <v>44700.37422266204</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C244" s="2">
+        <v>137.0</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F244" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G244" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J244" s="2">
+        <v>90.0</v>
+      </c>
+      <c r="K244" s="2">
+        <v>88.0</v>
+      </c>
+      <c r="L244" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M244" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N244" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O244" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P244" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R244" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S244" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="T244" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U244" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V244" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W244" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="X244" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="Z244" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA244" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB244" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC244" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>